<commit_message>
new report and excel
</commit_message>
<xml_diff>
--- a/hanoi pdbi results.xlsx
+++ b/hanoi pdbi results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/urielzaed/Documents/AI Search Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ran\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6024CD-331E-1F4E-967B-157CAB1961AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89469218-6378-4497-9C27-F551CF798ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{F418897E-E758-EE43-A2A2-5476BAC74443}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F418897E-E758-EE43-A2A2-5476BAC74443}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,12 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
-    <t>pdbi</t>
-  </si>
-  <si>
-    <t>additive</t>
-  </si>
-  <si>
     <t>1,7</t>
   </si>
   <si>
@@ -111,13 +105,19 @@
   </si>
   <si>
     <t>8,8</t>
+  </si>
+  <si>
+    <t>PDBI</t>
+  </si>
+  <si>
+    <t>Additive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -136,6 +136,14 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -174,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -183,6 +191,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -519,15 +533,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEFE0C76-50B8-1C4B-B189-A5BB97DAD60F}">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -539,7 +553,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -550,29 +564,34 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" ht="22" x14ac:dyDescent="0.2">
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" ht="21" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="1"/>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" ht="22" x14ac:dyDescent="0.2">
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" spans="1:14" ht="21" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -586,38 +605,40 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-    </row>
-    <row r="5" spans="1:13" ht="22" x14ac:dyDescent="0.2">
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
+      <c r="C5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>1</v>
+      <c r="G5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="22" x14ac:dyDescent="0.2">
+      <c r="L5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="5"/>
+    </row>
+    <row r="6" spans="1:14" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2">
         <v>36638</v>
@@ -627,7 +648,7 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G6" s="2">
         <v>1527</v>
@@ -638,7 +659,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L6" s="2">
         <v>2174</v>
@@ -646,11 +667,12 @@
       <c r="M6" s="2">
         <v>7364</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="22" x14ac:dyDescent="0.2">
+      <c r="N6" s="5"/>
+    </row>
+    <row r="7" spans="1:14" ht="21" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2">
         <v>11539</v>
@@ -660,7 +682,7 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G7" s="2">
         <v>548</v>
@@ -671,15 +693,16 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" ht="22" x14ac:dyDescent="0.2">
+      <c r="N7" s="5"/>
+    </row>
+    <row r="8" spans="1:14" ht="21" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" s="2">
         <v>8777</v>
@@ -689,7 +712,7 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G8" s="2">
         <v>482</v>
@@ -700,15 +723,16 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" ht="22" x14ac:dyDescent="0.2">
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" ht="21" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C9" s="2">
         <v>7198</v>
@@ -718,7 +742,7 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G9" s="2">
         <v>271</v>
@@ -729,15 +753,16 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" ht="22" x14ac:dyDescent="0.2">
+      <c r="N9" s="5"/>
+    </row>
+    <row r="10" spans="1:14" ht="21" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C10" s="2">
         <v>9564</v>
@@ -747,7 +772,7 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G10" s="2">
         <v>86</v>
@@ -758,15 +783,16 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" ht="22" x14ac:dyDescent="0.2">
+      <c r="N10" s="5"/>
+    </row>
+    <row r="11" spans="1:14" ht="21" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C11" s="2">
         <v>5559</v>
@@ -781,15 +807,16 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:13" ht="22" x14ac:dyDescent="0.2">
+      <c r="N11" s="5"/>
+    </row>
+    <row r="12" spans="1:14" ht="21" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2">
         <v>1561</v>
@@ -804,12 +831,13 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="1:13" ht="22" x14ac:dyDescent="0.2">
+      <c r="N12" s="5"/>
+    </row>
+    <row r="13" spans="1:14" ht="21" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -821,12 +849,13 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" ht="22" x14ac:dyDescent="0.2">
+      <c r="N13" s="5"/>
+    </row>
+    <row r="14" spans="1:14" ht="21" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -837,8 +866,12 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" ht="22" x14ac:dyDescent="0.2">
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+    </row>
+    <row r="15" spans="1:14" ht="21" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -850,7 +883,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="21" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -862,7 +895,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -874,7 +907,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -886,7 +919,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -898,7 +931,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -907,7 +940,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -916,7 +949,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -925,7 +958,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -934,7 +967,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -943,7 +976,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -952,7 +985,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -961,7 +994,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -970,7 +1003,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -979,7 +1012,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -988,7 +1021,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -997,7 +1030,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -1006,7 +1039,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1015,7 +1048,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1027,7 +1060,7 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1039,7 +1072,7 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1051,7 +1084,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1063,7 +1096,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1075,7 +1108,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1087,7 +1120,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>

</xml_diff>